<commit_message>
Revise the metadata files
</commit_message>
<xml_diff>
--- a/auto-fluorescence/latest/auto-fluorescence.xlsx
+++ b/auto-fluorescence/latest/auto-fluorescence.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="693">
   <si>
     <t>parent_id</t>
   </si>
@@ -1580,6 +1580,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>nanoPOTS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000246</t>
+  </si>
+  <si>
     <t>DESI</t>
   </si>
   <si>
@@ -1598,6 +1604,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
   </si>
   <si>
+    <t>snATAC-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000183</t>
+  </si>
+  <si>
     <t>Xenium</t>
   </si>
   <si>
@@ -1610,10 +1622,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>RNAseq (sc/sn)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000213</t>
+    <t>scRNA-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000248</t>
   </si>
   <si>
     <t>CosMx</t>
@@ -1664,6 +1676,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000160</t>
   </si>
   <si>
+    <t>snRNA-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000184</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -1712,6 +1730,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000197</t>
   </si>
   <si>
+    <t>scATAC-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000247</t>
+  </si>
+  <si>
     <t>Enhanced Stimulated Raman Spectroscopy (SRS)</t>
   </si>
   <si>
@@ -1730,12 +1754,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
   </si>
   <si>
-    <t>ATACseq (sc/sn)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000211</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -2258,7 +2276,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-08-03T09:16:15-07:00</t>
+    <t>2023-08-04T07:36:40-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2418,63 +2436,66 @@
         <v>455</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>678</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2">
+      <c r="H2" t="s">
+        <v>462</v>
+      </c>
       <c r="Z2" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +2507,7 @@
       <formula1>'operator'!$A$1:$A$203</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$11</formula1>
@@ -2552,42 +2573,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="B1" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="B2" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="B3" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="B4" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="B5" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -2605,18 +2626,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="B1" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -2634,34 +2655,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="B1" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>660</v>
+        <v>666</v>
       </c>
       <c r="B2" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="B3" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="B4" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -2679,34 +2700,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="B1" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="B2" t="s">
-        <v>670</v>
+        <v>676</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="B3" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="B4" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -2730,30 +2751,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="B1" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
       <c r="C1" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="D1" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="C2" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="D2" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
   </sheetData>
@@ -4581,7 +4602,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4849,6 +4870,30 @@
       </c>
       <c r="B33" t="s">
         <v>521</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>522</v>
+      </c>
+      <c r="B34" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>524</v>
+      </c>
+      <c r="B35" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>526</v>
+      </c>
+      <c r="B36" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4866,90 +4911,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="B1" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="B2" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B3" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="B4" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="B5" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="B6" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="B7" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="B9" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="B10" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="B11" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -4967,18 +5012,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="B1" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -4996,114 +5041,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="B1" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="B3" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="B4" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="B5" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="B6" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="B7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="B8" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="B9" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="B10" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="B11" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="B12" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="B13" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="B14" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -5121,242 +5166,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="B1" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="B2" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="B3" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="B4" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="B5" t="s">
-        <v>588</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="B7" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="B8" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="B9" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="B10" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="B11" t="s">
-        <v>600</v>
+        <v>606</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="B12" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="B13" t="s">
-        <v>604</v>
+        <v>610</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="B14" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="B15" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="B16" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="B17" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="B18" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="B19" t="s">
-        <v>616</v>
+        <v>622</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B20" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="B21" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="B22" t="s">
-        <v>622</v>
+        <v>628</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="B23" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="B24" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="B25" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="B26" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="B27" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="B28" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="B29" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="B30" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -5374,42 +5419,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="B1" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="B2" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="B3" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="B4" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="B5" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>